<commit_message>
POCOR-3533 - Improve on logic to check for principal and homeroom teacher edit comments for report cards
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="8600" yWindow="1380" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.comments","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "AssessmentItemResults.marks_formatted","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "AssessmentItemResults.education_subject_id"},"columns": {"matchFrom": "AssessmentPeriods.id","matchTo": "AssessmentItemResults.assessment_period_id"}}}</t>
-  </si>
-  <si>
     <t>${"repeatRows":{"displayValue":"AssessmentItems.education_subject.name"}}</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.comment_code_name","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "AssessmentItemResults.marks_formatted","type":"number","format":"2","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "AssessmentItemResults.education_subject_id"},"columns": {"matchFrom": "AssessmentPeriods.id","matchTo": "AssessmentItemResults.assessment_period_id"}}}</t>
   </si>
 </sst>
 </file>
@@ -614,6 +614,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -639,9 +642,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView view="pageLayout" topLeftCell="A8" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1197,7 +1197,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="26"/>
+      <c r="A1" s="27"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1206,10 +1206,10 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="26"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="1"/>
       <c r="C2" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -1217,7 +1217,7 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="26"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1238,15 +1238,15 @@
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
@@ -1255,15 +1255,15 @@
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="33"/>
+      <c r="B6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="24"/>
       <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -1272,15 +1272,15 @@
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
@@ -1289,15 +1289,15 @@
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
@@ -1306,10 +1306,10 @@
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1329,21 +1329,21 @@
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="24"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="12" t="s">
         <v>23</v>
       </c>
@@ -1353,10 +1353,10 @@
       <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="12" t="s">
         <v>25</v>
       </c>
@@ -1366,10 +1366,10 @@
       <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="12" t="s">
         <v>27</v>
       </c>
@@ -1388,15 +1388,15 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="15" t="s">
@@ -1406,10 +1406,10 @@
         <v>35</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>36</v>
@@ -1438,10 +1438,10 @@
         <v>43</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" customHeight="1">
@@ -1454,61 +1454,61 @@
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A20:G20"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="A20:G20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -1527,7 +1527,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1541,13 +1541,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16" t="s">
@@ -1568,13 +1568,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1597,7 +1597,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1611,7 +1611,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -1627,27 +1627,27 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
POCOR-3533 - Add total marks for report card template, fix bug on download behaviour where filetype is not correct, fix sorting for report card comments and statuses, fix subject comment tabs not showing properly, and fix finder names to camel case
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -4,13 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="1380" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="13660" yWindow="900" windowWidth="22820" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
     <sheet name="Competencies" sheetId="16" r:id="rId2"/>
     <sheet name="Assessments" sheetId="18" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Assessments!$A$1:$E$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Competencies!$A$1:$E$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$1:$G$23</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>${InstitutionClasses.name}</t>
   </si>
@@ -56,9 +61,6 @@
     <t>OpenEMIS ID:</t>
   </si>
   <si>
-    <t>Prinicipal:</t>
-  </si>
-  <si>
     <t>Student:</t>
   </si>
   <si>
@@ -200,9 +202,6 @@
     <t>${"match": {"displayValue": "StudentBehaviours.time_of_behaviour","type": "time","format":"H:i:s","rows": {"matchFrom": "StudentBehaviours.id","matchTo": "StudentBehaviours.id"}}}</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "StudentBehaviours.date_of_behaviour","type": "date","format":"d-m-Y","rows": {"matchFrom": "StudentBehaviours.id","matchTo": "StudentBehaviours.id"}}}</t>
-  </si>
-  <si>
     <t>${ReportCards.academic_period.name} - ${ReportCards.name}</t>
   </si>
   <si>
@@ -219,6 +218,18 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "AssessmentItemResults.marks_formatted","type":"number","format":"2","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "AssessmentItemResults.education_subject_id"},"columns": {"matchFrom": "AssessmentPeriods.id","matchTo": "AssessmentItemResults.assessment_period_id"}}}</t>
+  </si>
+  <si>
+    <t>Total Marks</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionSubjectStudents.total_mark","type":"number","format":"2","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionSubjectStudents.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>Principal:</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentBehaviours.date_of_behaviour","type": "date","format":"d/m/Y","rows": {"matchFrom": "StudentBehaviours.id","matchTo": "StudentBehaviours.id"}}}</t>
   </si>
 </sst>
 </file>
@@ -322,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -372,15 +383,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -392,7 +394,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -546,8 +548,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -562,16 +568,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,52 +592,68 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -654,7 +666,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -731,6 +743,8 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -807,6 +821,8 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1181,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A8" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1192,12 +1208,14 @@
     <col min="3" max="3" width="15.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="16" style="4" customWidth="1"/>
     <col min="5" max="5" width="28" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="11.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="27"/>
+      <c r="A1" s="31"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1206,18 +1224,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="31"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="27"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1226,170 +1244,170 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" ht="17" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="25" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="25" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="25" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="17" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -1399,63 +1417,63 @@
       <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="C17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="15" t="s">
+      <c r="F17" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="G17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="15" t="s">
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="12" t="s">
+      <c r="B18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="C18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="E18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>58</v>
+      <c r="F18" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -1465,30 +1483,30 @@
       <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26" t="s">
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="25" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1516,7 +1534,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
@@ -1524,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1535,47 +1553,54 @@
     <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="29" style="4" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="16" style="4" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12" t="s">
-        <v>52</v>
-      </c>
+      <c r="A3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1586,7 +1611,7 @@
   <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
@@ -1594,76 +1619,85 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="16.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="36" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="19" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="21" t="s">
+      <c r="E3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="22" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>44</v>
+      <c r="D4" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
POCOR-4156 - Adding the BMI to the report card. - BMI only get latest record within the report card start and end date. - BMI only support institution student. - Moved the logic to count the BMI to the beforeMarshall. - Adding association to the securityUsersTable.
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="13660" yWindow="900" windowWidth="22820" windowHeight="16060" tabRatio="500"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Assessments!$A$1:$E$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Competencies!$A$1:$E$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$1:$G$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>${InstitutionClasses.name}</t>
   </si>
@@ -230,6 +230,30 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "StudentBehaviours.date_of_behaviour","type": "date","format":"d/m/Y","rows": {"matchFrom": "StudentBehaviours.id","matchTo": "StudentBehaviours.id"}}}</t>
+  </si>
+  <si>
+    <t>Identity Number:</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student.identity_number}</t>
+  </si>
+  <si>
+    <t>Height:</t>
+  </si>
+  <si>
+    <t>Weight:</t>
+  </si>
+  <si>
+    <t>BMI:</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.body_mass.body_mass_index}</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.body_mass.height} m</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.body_mass.weight} kg</t>
   </si>
 </sst>
 </file>
@@ -394,7 +418,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="157">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -552,8 +576,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -626,39 +674,42 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,7 +717,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="157">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -745,6 +796,18 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -823,6 +886,18 @@
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1195,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:G22"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1215,7 +1290,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="31"/>
+      <c r="A1" s="27"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1224,7 +1299,7 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="31"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="1"/>
       <c r="C2" s="36" t="s">
         <v>58</v>
@@ -1235,7 +1310,7 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="31"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1295,10 +1370,10 @@
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="20" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
@@ -1312,221 +1387,256 @@
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="35"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="26"/>
       <c r="D9" s="20" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="1:7" ht="17" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="6"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="1:7" ht="17" customHeight="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="26" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="8" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="17" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+    <row r="15" spans="1:7">
+      <c r="A15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" customHeight="1">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="11" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="17" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F20" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G20" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="28" t="s">
+    <row r="21" spans="1:7" ht="16" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="26" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="26" t="s">
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -1636,22 +1746,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="14" t="s">

</xml_diff>

<commit_message>
POCOR-4148 - Update the default report card template with the competency period and item comments
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="13660" yWindow="900" windowWidth="22820" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
-    <sheet name="Competencies" sheetId="16" r:id="rId2"/>
-    <sheet name="Assessments" sheetId="18" r:id="rId3"/>
+    <sheet name="Competency Period Comments" sheetId="26" r:id="rId2"/>
+    <sheet name="Competency Item Comments" sheetId="25" r:id="rId3"/>
+    <sheet name="Competency Results" sheetId="16" r:id="rId4"/>
+    <sheet name="Assessments" sheetId="18" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Assessments!$A$1:$E$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Competencies!$A$1:$E$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Assessments!$A$1:$E$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Competency Item Comments'!$A$1:$D$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Competency Period Comments'!$A$1:$C$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Competency Results'!$A$1:$E$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>${InstitutionClasses.name}</t>
   </si>
@@ -70,9 +74,6 @@
     <t>Institution:</t>
   </si>
   <si>
-    <t>Competencies</t>
-  </si>
-  <si>
     <t>Template</t>
   </si>
   <si>
@@ -254,6 +255,27 @@
   </si>
   <si>
     <t>${InstitutionStudentsReportCards.body_mass.weight} kg</t>
+  </si>
+  <si>
+    <t>Competency Period Comments</t>
+  </si>
+  <si>
+    <t>Competency Item Comments</t>
+  </si>
+  <si>
+    <t>${"repeatRows":{"displayValue":"CompetencyTemplates.name","children":{"repeatRows":{"displayValue":"CompetencyPeriods.name","filter":"competency_template_id"}}}}</t>
+  </si>
+  <si>
+    <t>${"repeatRows":{"displayValue":"CompetencyTemplates.name","children":{"repeatRows":{"displayValue":"CompetencyPeriods.name","filter":"competency_template_id","children":{"repeatRows":{"displayValue":"CompetencyItems.name","filter":"competency_period_id"}}}}}}</t>
+  </si>
+  <si>
+    <t>${"match":{"displayValue":"StudentCompetencyPeriodComments.comments","rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyPeriodComments.competency_period_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match":{"displayValue":"StudentCompetencyItemComments.comments","rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyItemComments.competency_period_id","children":{"rows":{"matchFrom":"CompetencyItems.id","matchTo":"StudentCompetencyItemComments.competency_item_id","filter":"competency_period_id"}}}}}</t>
+  </si>
+  <si>
+    <t>Competency Results</t>
   </si>
 </sst>
 </file>
@@ -418,8 +440,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -674,42 +700,42 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -717,7 +743,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -808,6 +834,8 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -898,6 +926,8 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1273,7 +1303,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1290,7 +1320,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="27"/>
+      <c r="A1" s="32"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1299,18 +1329,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="C2" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="27"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1331,32 +1361,32 @@
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="35"/>
+        <v>65</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="36"/>
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23"/>
@@ -1365,15 +1395,15 @@
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>68</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>69</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
@@ -1382,15 +1412,15 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
@@ -1399,15 +1429,15 @@
       <c r="A9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
@@ -1416,15 +1446,15 @@
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="35"/>
+      <c r="B10" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="36"/>
       <c r="D10" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
@@ -1433,15 +1463,15 @@
       <c r="A11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>72</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>73</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
@@ -1456,23 +1486,23 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="A13" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1480,12 +1510,12 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -1493,12 +1523,12 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1516,7 +1546,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
@@ -1527,48 +1557,48 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>42</v>
-      </c>
       <c r="F20" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1">
@@ -1582,7 +1612,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
@@ -1592,38 +1622,33 @@
       <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="37" t="s">
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="28" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="A22:G22"/>
+  <mergeCells count="19">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
@@ -1637,6 +1662,12 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -1652,57 +1683,190 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="47" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="29" style="4" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="16" style="4" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1727,7 +1891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1747,7 +1911,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1756,7 +1920,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1765,36 +1929,36 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POCOR-4156 - Update name to StudentBodyMassesController and UserBodyMassesTable. - UserBodyMassesTable under User plugin. - Update db name to user_body_masses. - Update healthBehavior. - Update NavigationComponent. - Update MessageTrait. - Update report_card_template.
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -247,13 +247,13 @@
     <t>BMI:</t>
   </si>
   <si>
-    <t>${InstitutionStudentsReportCards.body_mass.body_mass_index}</t>
-  </si>
-  <si>
-    <t>${InstitutionStudentsReportCards.body_mass.height} m</t>
-  </si>
-  <si>
-    <t>${InstitutionStudentsReportCards.body_mass.weight} kg</t>
+    <t>${InstitutionStudentsReportCards.student_body_mass.height} m</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student_body_mass.weight} kg</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student_body_mass.body_mass_index}</t>
   </si>
 </sst>
 </file>
@@ -677,21 +677,24 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,9 +709,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1273,7 +1273,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1290,7 +1290,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="27"/>
+      <c r="A1" s="32"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1299,18 +1299,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="27"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1331,10 +1331,10 @@
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
@@ -1348,10 +1348,10 @@
       <c r="A6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
@@ -1365,10 +1365,10 @@
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="20" t="s">
         <v>68</v>
       </c>
@@ -1382,10 +1382,10 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>70</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
@@ -1416,15 +1416,15 @@
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="20" t="s">
         <v>71</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
@@ -1433,15 +1433,15 @@
       <c r="A11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="20" t="s">
         <v>72</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
@@ -1456,21 +1456,21 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
@@ -1480,10 +1480,10 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="8" t="s">
         <v>24</v>
       </c>
@@ -1493,10 +1493,10 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1592,38 +1592,33 @@
       <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="37" t="s">
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="37" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
@@ -1637,6 +1632,11 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -1669,13 +1669,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
POCOR-4156 - Update the report_card_template.
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -247,13 +247,13 @@
     <t>BMI:</t>
   </si>
   <si>
-    <t>${InstitutionStudentsReportCards.student_body_mass.height} m</t>
-  </si>
-  <si>
-    <t>${InstitutionStudentsReportCards.student_body_mass.weight} kg</t>
-  </si>
-  <si>
-    <t>${InstitutionStudentsReportCards.student_body_mass.body_mass_index}</t>
+    <t>${InstitutionStudentsReportCards.student.body_mass_index}</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student.weight} kg</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student.height} m</t>
   </si>
 </sst>
 </file>
@@ -677,38 +677,38 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1273,7 +1273,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1290,7 +1290,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="32"/>
+      <c r="A1" s="27"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1299,18 +1299,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="32"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="32"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1331,10 +1331,10 @@
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
@@ -1348,10 +1348,10 @@
       <c r="A6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
@@ -1365,10 +1365,10 @@
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="20" t="s">
         <v>68</v>
       </c>
@@ -1382,10 +1382,10 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>70</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
@@ -1416,10 +1416,10 @@
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="20" t="s">
         <v>71</v>
       </c>
@@ -1433,15 +1433,15 @@
       <c r="A11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="20" t="s">
         <v>72</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
@@ -1456,21 +1456,21 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
@@ -1480,10 +1480,10 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8" t="s">
         <v>24</v>
       </c>
@@ -1493,10 +1493,10 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1592,33 +1592,38 @@
       <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
@@ -1632,11 +1637,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -1669,13 +1669,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
POCOR-4148 - Update report card template for bmi
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -248,15 +248,6 @@
     <t>BMI:</t>
   </si>
   <si>
-    <t>${InstitutionStudentsReportCards.body_mass.body_mass_index}</t>
-  </si>
-  <si>
-    <t>${InstitutionStudentsReportCards.body_mass.height} m</t>
-  </si>
-  <si>
-    <t>${InstitutionStudentsReportCards.body_mass.weight} kg</t>
-  </si>
-  <si>
     <t>Competency Period Comments</t>
   </si>
   <si>
@@ -276,6 +267,15 @@
   </si>
   <si>
     <t>Competency Results</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student.height} m</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student.weight} kg</t>
+  </si>
+  <si>
+    <t>${InstitutionStudentsReportCards.student.body_mass_index}</t>
   </si>
 </sst>
 </file>
@@ -703,38 +703,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1320,7 +1320,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="32"/>
+      <c r="A1" s="27"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1329,18 +1329,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="32"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="32"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1361,10 +1361,10 @@
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
@@ -1378,10 +1378,10 @@
       <c r="A6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
@@ -1395,10 +1395,10 @@
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="20" t="s">
         <v>67</v>
       </c>
@@ -1412,10 +1412,10 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
@@ -1429,15 +1429,15 @@
       <c r="A9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="20" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
@@ -1446,15 +1446,15 @@
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="20" t="s">
         <v>70</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
@@ -1463,15 +1463,15 @@
       <c r="A11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="20" t="s">
         <v>71</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
@@ -1486,21 +1486,21 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1510,10 +1510,10 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8" t="s">
         <v>23</v>
       </c>
@@ -1523,10 +1523,10 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="8" t="s">
         <v>25</v>
       </c>
@@ -1622,33 +1622,38 @@
       <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
@@ -1663,11 +1668,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -1698,11 +1698,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="A1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -1717,11 +1717,11 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1762,12 +1762,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="A1" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -1785,12 +1785,12 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1833,13 +1833,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="A1" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
3.10.10 - Updated default template
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="13660" yWindow="900" windowWidth="22820" windowHeight="16060" tabRatio="500"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Competency Results'!$A$1:$E$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$1:$G$25</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>${InstitutionClasses.name}</t>
   </si>
@@ -276,6 +276,10 @@
   </si>
   <si>
     <t>${InstitutionStudentsReportCards.student.body_mass_index}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}
+</t>
   </si>
 </sst>
 </file>
@@ -627,7 +631,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -703,21 +707,24 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -733,14 +740,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="185">
@@ -933,49 +940,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>270932</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1041399</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>267547</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="270932" y="25400"/>
-          <a:ext cx="770467" cy="770467"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1302,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1320,7 +1284,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="27"/>
+      <c r="A1" s="40" t="s">
+        <v>82</v>
+      </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -1329,18 +1295,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="27"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1361,10 +1327,10 @@
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
@@ -1378,10 +1344,10 @@
       <c r="A6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
@@ -1395,10 +1361,10 @@
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="20" t="s">
         <v>67</v>
       </c>
@@ -1412,10 +1378,10 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
@@ -1429,10 +1395,10 @@
       <c r="A9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="20" t="s">
         <v>69</v>
       </c>
@@ -1446,10 +1412,10 @@
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="20" t="s">
         <v>70</v>
       </c>
@@ -1463,10 +1429,10 @@
       <c r="A11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="20" t="s">
         <v>71</v>
       </c>
@@ -1486,21 +1452,21 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1510,10 +1476,10 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="8" t="s">
         <v>23</v>
       </c>
@@ -1523,10 +1489,10 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="8" t="s">
         <v>25</v>
       </c>
@@ -1622,38 +1588,33 @@
       <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="37" t="s">
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="37" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
@@ -1668,11 +1629,15 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1698,11 +1663,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -1762,12 +1727,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -1833,13 +1798,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
POCOR- Include learning outcome into report card . Make changes to report_card.template to add placeholder for learning outcome(Outcome Subject Comment & Outcome Result)
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="900" windowWidth="22820" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="12760" yWindow="2560" windowWidth="22820" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="Competency Item Comments" sheetId="25" r:id="rId3"/>
     <sheet name="Competency Results" sheetId="16" r:id="rId4"/>
     <sheet name="Assessments" sheetId="18" r:id="rId5"/>
+    <sheet name="Outcome Subject Comments" sheetId="27" r:id="rId6"/>
+    <sheet name="Outcome Result" sheetId="28" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Assessments!$A$1:$E$5</definedName>
@@ -19,6 +21,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Competency Period Comments'!$A$1:$C$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Competency Results'!$A$1:$E$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$1:$G$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Outcome Result'!$A$1:$E$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Outcome Subject Comments'!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>${InstitutionClasses.name}</t>
   </si>
@@ -180,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">Assessments </t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentCompetencyResults.competency_grading_option.name","rows": {"matchFrom": "CompetencyPeriods.id","matchTo": "StudentCompetencyResults.competency_period_id","children": {"rows": {"matchFrom": "CompetencyCriterias.id","matchTo": "StudentCompetencyResults.competency_criteria_id","filter":"competency_period_id"}}}}}</t>
   </si>
   <si>
     <t>${InstitutionStudentsReportCards.student.name}</t>
@@ -280,6 +281,27 @@
   <si>
     <t xml:space="preserve">${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}
 </t>
+  </si>
+  <si>
+    <t>Outcome Subject Comments</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>${"repeatRows":{"displayValue":"OutcomeTemplates.name","children":{"repeatRows":{"displayValue":"OutcomePeriods.name","filter":"outcome_template_id","children":{"repeatRows":{"displayValue":"OutcomeSubjects.name","filter":"outcome_period_id"}}}}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"repeatRows":{"displayValue":"OutcomeTemplates.name","children":{"repeatRows":{"displayValue":"OutcomePeriods.name","filter":"outcome_template_id", "children":{"repeatRows":{"displayValue":"OutcomeSubjects.name", "filter":"outcome_period_id", "children":{"repeatRows":{"displayValue":"OutcomeCriterias.name","filter":"outcome_subject_id"}}}}}}}}  </t>
+  </si>
+  <si>
+    <t>${"match":{"displayValue":"StudentOutcomeResults.outcome_grading_option.name","rows":{"matchFrom":"OutcomeTemplates.id","matchTo":"StudentOutcomeResults.outcome_template_id","children":{"rows":{"matchFrom":"OutcomePeriods.id","matchTo":"StudentOutcomeResults.outcome_period_id","filter":"outcome_template_id","children":{"rows":{"matchFrom":"OutcomeSubjects.education_subject_id","matchTo":"StudentOutcomeResults.education_subject_id","filter":"outcome_period_id","children":{"rows":{"matchFrom":"OutcomeCriterias.id","matchTo":"StudentOutcomeResults.outcome_criteria_id","filter":"outcome_subject_id"}}}}}}}}}</t>
+  </si>
+  <si>
+    <t>${"match":{"displayValue":"StudentOutcomeSubjectComments.comments","rows":{"matchFrom":"OutcomeTemplates.id","matchTo":"StudentOutcomeSubjectComments.outcome_template_id","children":{"rows":{"matchFrom":"OutcomePeriods.id","matchTo":"StudentOutcomeSubjectComments.outcome_period_id","filter":"outcome_template_id","children":{"rows":{"matchFrom":"OutcomeSubjects.education_subject_id","matchTo":"StudentOutcomeSubjectComments.education_subject_id","filter":"outcome_period_id"}}}}}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentCompetencyResults.competency_grading_option.name","rows": {"matchFrom": "CompetencyPeriods.id","matchTo": "StudentCompetencyResults.competency_period_id","children": {"rows": {"matchFrom": "CompetencyCriterias.id","matchTo": "StudentCompetencyResults.competency_criteria_id","filter":"competency_period_id"}}}}}</t>
   </si>
 </sst>
 </file>
@@ -631,7 +653,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -707,6 +729,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -723,6 +748,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -745,9 +773,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="185">
@@ -1266,7 +1291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -1284,8 +1309,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="40" t="s">
-        <v>82</v>
+      <c r="A1" s="33" t="s">
+        <v>81</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1295,18 +1320,18 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="26" customHeight="1">
-      <c r="A2" s="32"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
-      <c r="A3" s="32"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1327,32 +1352,32 @@
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="36"/>
+        <v>64</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="38"/>
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23"/>
@@ -1361,15 +1386,15 @@
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
@@ -1378,15 +1403,15 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
@@ -1395,15 +1420,15 @@
       <c r="A9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
@@ -1412,15 +1437,15 @@
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="36"/>
+      <c r="B10" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="38"/>
       <c r="D10" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
@@ -1429,15 +1454,15 @@
       <c r="A11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
@@ -1452,21 +1477,21 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1476,10 +1501,10 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8" t="s">
         <v>23</v>
       </c>
@@ -1489,10 +1514,10 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="8" t="s">
         <v>25</v>
       </c>
@@ -1511,15 +1536,15 @@
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
@@ -1529,10 +1554,10 @@
         <v>33</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>34</v>
@@ -1561,10 +1586,10 @@
         <v>41</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1">
@@ -1577,41 +1602,41 @@
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -1663,11 +1688,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="A1" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -1682,11 +1707,11 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1727,12 +1752,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="A1" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -1750,12 +1775,12 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1798,13 +1823,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="A1" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
@@ -1825,13 +1850,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1875,22 +1900,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="14" t="s">
@@ -1900,7 +1925,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>45</v>
@@ -1914,13 +1939,13 @@
         <v>43</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>42</v>
@@ -1940,4 +1965,151 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="47" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-4508 - Added placeholders for subject comments in Outcome Results tab in the default report card template.
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2140" windowWidth="25600" windowHeight="15620" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="6480" yWindow="2140" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Competency Results" sheetId="4" r:id="rId4"/>
     <sheet name="Assessments" sheetId="5" r:id="rId5"/>
     <sheet name="Outcome Subject Comments" sheetId="6" r:id="rId6"/>
-    <sheet name="Outcome Result" sheetId="7" r:id="rId7"/>
+    <sheet name="Outcome Results" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
   <si>
     <t>Competency Item Comments</t>
   </si>
@@ -345,6 +345,12 @@
   <si>
     <t>${"match":{"displayValue":"StudentCompetencyItemComments.comments","rows":{"matchFrom":"CompetencyTemplates.id","matchTo":"StudentCompetencyItemComments.competency_template_id","children":{"rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyItemComments.competency_period_id","filter":"competency_template_id","children":{"rows":{"matchFrom":"CompetencyItems.id","matchTo":"StudentCompetencyItemComments.competency_item_id","filter":"competency_period_id","mergeBy":{"mergeFrom":"CompetencyCriterias.id","filter":"competency_item_id"}}}}}}}}</t>
   </si>
+  <si>
+    <t>Subject Comments</t>
+  </si>
+  <si>
+    <t>${"match":{"displayValue":"StudentOutcomeSubjectComments.comments","rows":{"matchFrom":"OutcomeTemplates.id","matchTo":"StudentOutcomeSubjectComments.outcome_template_id","children":{"rows":{"matchFrom":"OutcomePeriods.id","matchTo":"StudentOutcomeSubjectComments.outcome_period_id","filter":"outcome_template_id","children":{"rows":{"matchFrom":"OutcomeSubjects.education_subject_id","matchTo":"StudentOutcomeSubjectComments.education_subject_id","filter":"outcome_period_id","mergeBy":{"mergeFrom":"OutcomeCriterias.id","filter":"outcome_subject_id"}}}}}}}}</t>
+  </si>
 </sst>
 </file>
 
@@ -419,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -540,13 +546,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -610,25 +633,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -636,8 +651,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -645,16 +671,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -986,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -1003,7 +1031,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1"/>
@@ -1024,14 +1052,14 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="37"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="6"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1045,7 +1073,7 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="37"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1086,10 +1114,10 @@
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
@@ -1113,10 +1141,10 @@
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
@@ -1140,10 +1168,10 @@
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
@@ -1167,10 +1195,10 @@
       <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
@@ -1194,10 +1222,10 @@
       <c r="A9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="11" t="s">
         <v>30</v>
       </c>
@@ -1221,10 +1249,10 @@
       <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="11" t="s">
         <v>34</v>
       </c>
@@ -1248,10 +1276,10 @@
       <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="11" t="s">
         <v>38</v>
       </c>
@@ -1275,10 +1303,10 @@
       <c r="A12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="11" t="s">
         <v>42</v>
       </c>
@@ -1302,10 +1330,10 @@
       <c r="A13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18"/>
       <c r="F13" s="13"/>
@@ -1325,10 +1353,10 @@
       <c r="A14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18"/>
       <c r="F14" s="13"/>
@@ -1364,11 +1392,11 @@
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="38" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="30"/>
-      <c r="C16" s="28"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -1385,10 +1413,10 @@
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="34"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="25" t="s">
         <v>59</v>
       </c>
@@ -1408,10 +1436,10 @@
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="25" t="s">
         <v>70</v>
       </c>
@@ -1431,10 +1459,10 @@
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="34"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="25" t="s">
         <v>72</v>
       </c>
@@ -1454,10 +1482,10 @@
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="25" t="s">
         <v>74</v>
       </c>
@@ -1496,7 +1524,7 @@
       <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="29" t="s">
         <v>75</v>
       </c>
       <c r="B22" s="30"/>
@@ -1504,7 +1532,7 @@
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="28"/>
+      <c r="G22" s="31"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -1602,7 +1630,7 @@
       <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="30"/>
@@ -1610,7 +1638,7 @@
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
-      <c r="G26" s="28"/>
+      <c r="G26" s="31"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -1623,17 +1651,17 @@
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="39" t="s">
         <v>91</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="28"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -1646,17 +1674,17 @@
       <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="39" t="s">
         <v>93</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
-      <c r="G28" s="28"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -2660,6 +2688,13 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A26:G26"/>
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:F2"/>
@@ -2672,17 +2707,10 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A26:G26"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2710,11 +2738,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="30"/>
-      <c r="C1" s="28"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -4048,12 +4076,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -5394,7 +5422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5412,16 +5440,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -5476,10 +5504,10 @@
       <c r="F3" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="28" t="s">
         <v>104</v>
       </c>
       <c r="I3" s="3"/>
@@ -6809,13 +6837,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="28"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -6828,13 +6856,13 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
-      <c r="E2" s="28"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -8202,12 +8230,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -9549,7 +9577,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -9559,19 +9587,19 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="37.83203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
     <col min="7" max="15" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -9598,7 +9626,9 @@
       <c r="E2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -9619,7 +9649,9 @@
       <c r="E3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="44" t="s">
+        <v>107</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -10917,7 +10949,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
POCOR-4528 - Fixed placeholders for Comments in Competency Period Comments and Competency Item Comments
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2140" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="10640" yWindow="2480" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>Institution:</t>
   </si>
   <si>
-    <t>${"match":{"displayValue":"StudentCompetencyPeriodComments.comments","rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyPeriodComments.competency_period_id"}}}</t>
-  </si>
-  <si>
     <t>${Institutions.code_name}</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
   </si>
   <si>
     <t>${"repeatRows":{"displayValue":"CompetencyTemplates.name","children":{"repeatRows":{"displayValue":"CompetencyPeriods.name","filter":"competency_template_id","children":{"repeatRows":{"displayValue":"CompetencyItems.name","filter":"competency_period_id"}}}}}}</t>
-  </si>
-  <si>
-    <t>${"match":{"displayValue":"StudentCompetencyItemComments.comments","rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyItemComments.competency_period_id","children":{"rows":{"matchFrom":"CompetencyItems.id","matchTo":"StudentCompetencyItemComments.competency_item_id","filter":"competency_period_id"}}}}}</t>
   </si>
   <si>
     <t>Student:</t>
@@ -351,6 +345,13 @@
   <si>
     <t>${"match":{"displayValue":"StudentOutcomeSubjectComments.comments","rows":{"matchFrom":"OutcomeTemplates.id","matchTo":"StudentOutcomeSubjectComments.outcome_template_id","children":{"rows":{"matchFrom":"OutcomePeriods.id","matchTo":"StudentOutcomeSubjectComments.outcome_period_id","filter":"outcome_template_id","children":{"rows":{"matchFrom":"OutcomeSubjects.education_subject_id","matchTo":"StudentOutcomeSubjectComments.education_subject_id","filter":"outcome_period_id","mergeBy":{"mergeFrom":"OutcomeCriterias.id","filter":"outcome_subject_id"}}}}}}}}</t>
   </si>
+  <si>
+    <t xml:space="preserve">${"match":{"displayValue":"StudentCompetencyPeriodComments.comments","rows":{"matchFrom":"CompetencyTemplates.id","matchTo":"StudentCompetencyPeriodComments.competency_template_id","children":{"rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyPeriodComments.competency_period_id","filter":"competency_template_id"}}}}}
+</t>
+  </si>
+  <si>
+    <t>${"match":{"displayValue":"StudentCompetencyItemComments.comments","rows":{"matchFrom":"CompetencyTemplates.id","matchTo":"StudentCompetencyItemComments.competency_template_id","children":{"rows":{"matchFrom":"CompetencyPeriods.id","matchTo":"StudentCompetencyItemComments.competency_period_id","filter":"competency_template_id","children":{"rows":{"matchFrom":"CompetencyItems.id","matchTo":"StudentCompetencyItemComments.competency_item_id","filter":"competency_period_id"}}}}}}}</t>
+  </si>
 </sst>
 </file>
 
@@ -569,7 +570,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -639,11 +640,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -651,19 +664,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -674,8 +678,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1031,7 +1035,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1"/>
@@ -1052,14 +1056,14 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="33"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="6"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1073,7 +1077,7 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="33"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1114,15 +1118,15 @@
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>10</v>
+      <c r="B5" s="30" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="3"/>
@@ -1139,17 +1143,17 @@
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="3"/>
@@ -1166,17 +1170,17 @@
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="3"/>
@@ -1193,17 +1197,17 @@
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3"/>
@@ -1220,17 +1224,17 @@
     </row>
     <row r="9" spans="1:17" ht="12" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="3"/>
@@ -1247,17 +1251,17 @@
     </row>
     <row r="10" spans="1:17" ht="12" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="3"/>
@@ -1274,17 +1278,17 @@
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="3"/>
@@ -1301,17 +1305,17 @@
     </row>
     <row r="12" spans="1:17" ht="12" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="3"/>
@@ -1328,10 +1332,10 @@
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="17"/>
@@ -1351,10 +1355,10 @@
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="17"/>
@@ -1392,10 +1396,10 @@
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="30"/>
+      <c r="A16" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="33"/>
       <c r="C16" s="31"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1413,12 +1417,12 @@
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="37"/>
+      <c r="A17" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="40"/>
       <c r="C17" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
@@ -1436,12 +1440,12 @@
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="37"/>
+      <c r="A18" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="40"/>
       <c r="C18" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
@@ -1459,12 +1463,12 @@
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="37"/>
+      <c r="A19" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="40"/>
       <c r="C19" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
@@ -1482,12 +1486,12 @@
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="37"/>
+      <c r="A20" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="40"/>
       <c r="C20" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
@@ -1524,14 +1528,14 @@
       <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="A22" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
       <c r="G22" s="31"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1546,25 +1550,25 @@
     </row>
     <row r="23" spans="1:17" ht="12" customHeight="1">
       <c r="A23" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="D23" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="E23" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="F23" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="G23" s="24" t="s">
         <v>80</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1579,25 +1583,25 @@
     </row>
     <row r="24" spans="1:17" ht="12" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1630,14 +1634,14 @@
       <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
       <c r="G26" s="31"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1651,16 +1655,16 @@
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="40" t="s">
-        <v>90</v>
+      <c r="A27" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="B27" s="31"/>
-      <c r="C27" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
+      <c r="C27" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="31"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1674,16 +1678,16 @@
       <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="40" t="s">
-        <v>92</v>
+      <c r="A28" s="34" t="s">
+        <v>90</v>
       </c>
       <c r="B28" s="31"/>
-      <c r="C28" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
+      <c r="C28" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
       <c r="G28" s="31"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -2688,6 +2692,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="C27:G27"/>
@@ -2696,21 +2710,11 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2726,7 +2730,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -2738,10 +2744,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="31"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2780,8 +2786,8 @@
         <v>7</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
+      <c r="C3" s="45" t="s">
+        <v>106</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -4062,7 +4068,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4076,11 +4082,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="31"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -4101,7 +4107,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -4119,12 +4125,12 @@
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -5440,16 +5446,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="A1" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -5466,22 +5472,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>101</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>103</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -5493,22 +5499,22 @@
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -6837,12 +6843,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="31"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -6856,12 +6862,12 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="31"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -6876,19 +6882,19 @@
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
       <c r="A3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="E3" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>63</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -6903,19 +6909,19 @@
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1">
       <c r="A4" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -8230,11 +8236,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="31"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -8255,7 +8261,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -8273,12 +8279,12 @@
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -9592,14 +9598,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="A1" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -9618,16 +9624,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -9641,16 +9647,16 @@
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>107</v>
+        <v>97</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>

</xml_diff>

<commit_message>
POCOR-5814:subject name showing in institution_subjects table|status:Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -349,7 +349,7 @@
     <t xml:space="preserve">Additional comments</t>
   </si>
   <si>
-    <t xml:space="preserve">${"repeatRows":{"displayValue":"AssessmentItems.education_subject.name"}}</t>
+    <t xml:space="preserve">${"repeatRows":{"displayValue":"InstitutionSubjectStudentsWithName.institution_subject.name"}}</t>
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "SubjectTeacher.name","rows": {"matchFrom": "SubjectTeacher.education_subject_id","matchTo": "SubjectTeacher.education_subject_id"}}}</t>
@@ -408,6 +408,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -429,6 +430,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -436,6 +438,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -443,6 +446,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -450,18 +454,21 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF2A3238"/>
       <name val="lato_regular"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -545,7 +552,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,7 +572,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -683,12 +690,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -760,7 +767,7 @@
   </sheetPr>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2523,7 +2530,7 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2595,276 +2602,24 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-    </row>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3850,7 +3605,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -3865,7 +3620,7 @@
   </sheetPr>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3943,294 +3698,24 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5216,7 +4701,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -5231,7 +4716,7 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5329,312 +4814,24 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-    </row>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6620,7 +5817,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -6635,8 +5832,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6752,312 +5949,23 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-    </row>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8044,7 +6952,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -8059,7 +6967,7 @@
   </sheetPr>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8137,294 +7045,24 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9410,7 +8048,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -9425,7 +8063,7 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -9513,312 +8151,24 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-    </row>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10804,7 +9154,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
POCOR:6810: code enhance for subject placeholder in assessment tab | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poona\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CC27BA-0563-4CC5-AA74-E8603F13D81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -354,9 +348,6 @@
     <t>Additional comments</t>
   </si>
   <si>
-    <t>${"repeatRows":{"displayValue":"InstitutionSubjectStudentsWithName.institution_subject.name"}}</t>
-  </si>
-  <si>
     <t>Outcome Subject Comments</t>
   </si>
   <si>
@@ -397,12 +388,15 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.comments","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.education_subject_id","matchTo": "InstitutionSubjectStudentsWithName.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.name","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -524,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -590,6 +584,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -597,25 +604,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -746,7 +743,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -778,27 +775,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -830,24 +809,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1023,27 +984,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q999"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.58203125" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
     <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
     <col min="5" max="5" width="27.75" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="17" width="10.33203125" customWidth="1"/>
+    <col min="8" max="17" width="10.375" customWidth="1"/>
     <col min="18" max="26" width="11" customWidth="1"/>
     <col min="27" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -1064,14 +1025,14 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="31"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="5"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1085,7 +1046,7 @@
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="31"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1126,10 +1087,10 @@
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1153,10 +1114,10 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1180,10 +1141,10 @@
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
@@ -1207,10 +1168,10 @@
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1234,10 +1195,10 @@
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="12" t="s">
         <v>20</v>
       </c>
@@ -1261,10 +1222,10 @@
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
@@ -1288,10 +1249,10 @@
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
@@ -1315,10 +1276,10 @@
       <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
@@ -1342,10 +1303,10 @@
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="12" t="s">
         <v>36</v>
       </c>
@@ -1369,10 +1330,10 @@
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="12" t="s">
         <v>40</v>
       </c>
@@ -1412,11 +1373,11 @@
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1433,10 +1394,10 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="16" t="s">
         <v>44</v>
       </c>
@@ -1456,10 +1417,10 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="16" t="s">
         <v>46</v>
       </c>
@@ -1479,10 +1440,10 @@
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="16" t="s">
         <v>48</v>
       </c>
@@ -1502,10 +1463,10 @@
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="16" t="s">
         <v>50</v>
       </c>
@@ -1544,15 +1505,15 @@
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1650,15 +1611,15 @@
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1671,17 +1632,17 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="30"/>
+      <c r="C27" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1694,17 +1655,17 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1737,11 +1698,11 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
@@ -2745,21 +2706,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="A31:C31"/>
@@ -2769,6 +2715,21 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2780,28 +2741,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.08203125" customWidth="1"/>
-    <col min="2" max="2" width="21.58203125" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="13" width="10.33203125" customWidth="1"/>
+    <col min="7" max="13" width="10.375" customWidth="1"/>
     <col min="14" max="26" width="11" customWidth="1"/>
     <col min="27" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -3864,30 +3825,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="46.58203125" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
     <col min="5" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="14" width="10.33203125" customWidth="1"/>
+    <col min="7" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="26" width="11" customWidth="1"/>
     <col min="27" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -4954,22 +4915,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
     <col min="6" max="6" width="31.25" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="22.75" customWidth="1"/>
-    <col min="9" max="15" width="10.33203125" customWidth="1"/>
+    <col min="9" max="15" width="10.375" customWidth="1"/>
     <col min="16" max="26" width="11" customWidth="1"/>
     <col min="27" max="1025" width="10.5" customWidth="1"/>
   </cols>
@@ -6064,35 +6025,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="16.58203125" customWidth="1"/>
+    <col min="1" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="22.75" customWidth="1"/>
-    <col min="6" max="6" width="20.58203125" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
     <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="16" width="10.33203125" customWidth="1"/>
+    <col min="8" max="16" width="10.375" customWidth="1"/>
     <col min="17" max="27" width="11" customWidth="1"/>
     <col min="28" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -6156,22 +6117,22 @@
     </row>
     <row r="4" spans="1:16" ht="12" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>121</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -7195,30 +7156,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="46.58203125" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
     <col min="5" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="14" width="10.33203125" customWidth="1"/>
+    <col min="7" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="26" width="11" customWidth="1"/>
     <col min="27" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -7238,7 +7199,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>66</v>
@@ -7256,12 +7217,12 @@
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -8285,27 +8246,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" customWidth="1"/>
-    <col min="7" max="15" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="15" width="10.375" customWidth="1"/>
     <col min="16" max="26" width="11" customWidth="1"/>
     <col min="27" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -8330,7 +8291,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>89</v>
@@ -8339,7 +8300,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -8353,16 +8314,16 @@
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>

</xml_diff>

<commit_message>
POCOR-5227: code enhancement in Institution > performance > report card | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umairah/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266F5220-3794-6345-ADF4-4CF848854156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="16380" windowHeight="8205" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Outcome Subject Comments" sheetId="6" r:id="rId6"/>
     <sheet name="Outcome Results" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -410,12 +404,27 @@
   </si>
   <si>
     <t>Institution Subjects</t>
+  </si>
+  <si>
+    <t>Teacher Commented OpenemisNo</t>
+  </si>
+  <si>
+    <t>Teacher Commented Name</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_openemis_no","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_name","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "SubjectTeacher.name","rows": {"matchFrom": "SubjectTeacher.education_subject_id","matchTo": "SubjectTeacher.education_subject_id"}}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -537,36 +546,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -631,7 +612,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,7 +768,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -814,7 +820,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1008,765 +1014,765 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="8" max="17" width="10.33203125" customWidth="1"/>
+    <col min="8" max="17" width="10.375" customWidth="1"/>
     <col min="18" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" ht="12" customHeight="1">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="22" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="12" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="22" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" ht="12" customHeight="1">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="22" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="26" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="26" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="26" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="26" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" ht="12" customHeight="1">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G23" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" ht="12" customHeight="1">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="25"/>
+      <c r="C28" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" ht="12" customHeight="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="18" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B35" s="30"/>
+      <c r="B35" s="20"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="19" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2735,6 +2741,21 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="A31:C31"/>
@@ -2744,21 +2765,6 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:G27"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2770,77 +2776,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
-    <col min="4" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="13" width="10.33203125" customWidth="1"/>
+    <col min="4" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="13" width="10.375" customWidth="1"/>
     <col min="14" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="12" customHeight="1"/>
     <row r="5" spans="1:13" ht="12" customHeight="1"/>
@@ -3853,83 +3859,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="14" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
+    <col min="5" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1"/>
     <row r="5" spans="1:14" ht="12" customHeight="1"/>
@@ -4942,105 +4948,105 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="31.125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="15" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.625" customWidth="1"/>
+    <col min="9" max="15" width="10.375" customWidth="1"/>
     <col min="16" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1"/>
     <row r="5" spans="1:15" ht="12" customHeight="1"/>
@@ -6053,127 +6059,139 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="16" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.625" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.75" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="16" width="10.375" customWidth="1"/>
     <col min="17" max="27" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
+      <c r="H3" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="E4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="F4" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="G4" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="H4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1"/>
     <row r="6" spans="1:17" ht="12" customHeight="1"/>
@@ -7177,7 +7195,7 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -7186,83 +7204,83 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="14" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
+    <col min="5" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1"/>
     <row r="5" spans="1:14" ht="12" customHeight="1"/>
@@ -8275,93 +8293,93 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="15" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="15" width="10.375" customWidth="1"/>
     <col min="16" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1"/>
     <row r="5" spans="1:15" ht="12" customHeight="1"/>

</xml_diff>

<commit_message>
POCOR-7031: Template update STATUS:Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehteramahmad/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621FD50E-19DA-7246-8274-C15B7E266AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="16380" windowHeight="8205" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Outcome Subject Comments" sheetId="6" r:id="rId6"/>
     <sheet name="Outcome Results" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,6 +24,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -40,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -99,6 +94,9 @@
     <t>Principal:</t>
   </si>
   <si>
+    <t>${Principal.user.name}</t>
+  </si>
+  <si>
     <t>Nationality:</t>
   </si>
   <si>
@@ -120,6 +118,9 @@
     <t>Homeroom Teacher:</t>
   </si>
   <si>
+    <t>${InstitutionClasses.staff.name}</t>
+  </si>
+  <si>
     <t>Date of Birth:</t>
   </si>
   <si>
@@ -405,16 +406,25 @@
     <t>Institution Subjects</t>
   </si>
   <si>
-    <t xml:space="preserve">${Principal.user.name}, ${Principal.user.preferred_name}	</t>
-  </si>
-  <si>
-    <t>${InstitutionClasses.staff.name},${InstitutionClasses.staff.preferred_name}</t>
+    <t>Teacher Commented OpenemisNo</t>
+  </si>
+  <si>
+    <t>Teacher Commented Name</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_openemis_no","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_name","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "SubjectTeacher.name","rows": {"matchFrom": "SubjectTeacher.education_subject_id","matchTo": "SubjectTeacher.education_subject_id"}}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -536,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -601,9 +611,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -761,7 +768,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -813,7 +820,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1007,34 +1014,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="8" max="17" width="10.33203125" customWidth="1"/>
+    <col min="8" max="17" width="10.375" customWidth="1"/>
     <col min="18" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -1055,14 +1060,14 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="32"/>
+      <c r="A2" s="31"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="5"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1076,7 +1081,7 @@
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="32"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1117,10 +1122,10 @@
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1144,10 +1149,10 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1171,10 +1176,10 @@
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="31"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
@@ -1198,10 +1203,10 @@
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1225,15 +1230,15 @@
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="31"/>
+      <c r="B9" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="30"/>
       <c r="D9" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="4"/>
@@ -1250,17 +1255,17 @@
     </row>
     <row r="10" spans="1:17" ht="12" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="B10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="30"/>
       <c r="D10" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="4"/>
@@ -1277,17 +1282,17 @@
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="31"/>
+        <v>26</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="30"/>
       <c r="D11" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="4"/>
@@ -1304,17 +1309,17 @@
     </row>
     <row r="12" spans="1:17" ht="12" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="31"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="30"/>
       <c r="D12" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="4"/>
@@ -1331,17 +1336,17 @@
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="31"/>
+        <v>34</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="30"/>
       <c r="D13" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="4"/>
@@ -1358,17 +1363,17 @@
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="31"/>
+        <v>38</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="30"/>
       <c r="D14" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="4"/>
@@ -1403,11 +1408,11 @@
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1424,12 +1429,12 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="29"/>
+      <c r="A17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="28"/>
       <c r="C17" s="16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -1447,12 +1452,12 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="29"/>
+      <c r="A18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="28"/>
       <c r="C18" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1470,12 +1475,12 @@
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="29"/>
+      <c r="A19" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="28"/>
       <c r="C19" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1493,12 +1498,12 @@
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="29"/>
+      <c r="A20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="28"/>
       <c r="C20" s="16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -1535,15 +1540,15 @@
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="A22" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1557,25 +1562,25 @@
     </row>
     <row r="23" spans="1:17" ht="12" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -1590,25 +1595,25 @@
     </row>
     <row r="24" spans="1:17" ht="12" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1641,15 +1646,15 @@
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
+      <c r="A26" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1662,17 +1667,17 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
+      <c r="A27" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1685,17 +1690,17 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
+      <c r="A28" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1728,32 +1733,32 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
@@ -1765,10 +1770,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1"/>
@@ -2771,27 +2776,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
-    <col min="4" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="13" width="10.33203125" customWidth="1"/>
+    <col min="4" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="13" width="10.375" customWidth="1"/>
     <col min="14" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -2805,13 +2810,13 @@
     </row>
     <row r="2" spans="1:13" ht="12" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -2826,11 +2831,11 @@
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3854,29 +3859,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="14" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
+    <col min="5" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -3890,16 +3895,16 @@
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -3914,12 +3919,12 @@
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -4943,38 +4948,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="31.125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="15" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.625" customWidth="1"/>
+    <col min="9" max="15" width="10.375" customWidth="1"/>
     <col min="16" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -4985,28 +4990,28 @@
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -5018,22 +5023,22 @@
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -6054,34 +6059,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="16" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.625" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.75" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="16" width="10.375" customWidth="1"/>
     <col min="17" max="27" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -6094,14 +6101,14 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1">
-      <c r="A2" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="A2" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -6115,28 +6122,32 @@
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+        <v>105</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>124</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -6147,27 +6158,33 @@
       <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1">
-      <c r="A4" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="B4" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="C4" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="F4" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -7178,7 +7195,7 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -7187,29 +7204,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="14" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
+    <col min="5" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -7223,16 +7240,16 @@
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -7247,12 +7264,12 @@
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -8276,32 +8293,32 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="15" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="15" width="10.375" customWidth="1"/>
     <col min="16" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -8314,22 +8331,22 @@
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -8343,16 +8360,16 @@
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>

</xml_diff>

<commit_message>
POCOR-7033: Develop gender placeholder in student report card STATUS:Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umairah/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehteramahmad/Sites/testingPurpose/repositories/pocor/pocor-openemis-core/webroot/export/customexcel/default_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266F5220-3794-6345-ADF4-4CF848854156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E193C2D5-6C7D-5842-89B8-E80C5BD3ABA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,18 +21,8 @@
     <sheet name="Outcome Subject Comments" sheetId="6" r:id="rId6"/>
     <sheet name="Outcome Results" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -41,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -100,9 +90,6 @@
     <t>Principal:</t>
   </si>
   <si>
-    <t>${Principal.user.name}</t>
-  </si>
-  <si>
     <t>Nationality:</t>
   </si>
   <si>
@@ -124,9 +111,6 @@
     <t>Homeroom Teacher:</t>
   </si>
   <si>
-    <t>${InstitutionClasses.staff.name}</t>
-  </si>
-  <si>
     <t>Date of Birth:</t>
   </si>
   <si>
@@ -410,6 +394,27 @@
   </si>
   <si>
     <t>Institution Subjects</t>
+  </si>
+  <si>
+    <t>Teacher Commented OpenemisNo</t>
+  </si>
+  <si>
+    <t>Teacher Commented Name</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_openemis_no","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_name","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "SubjectTeacher.name","rows": {"matchFrom": "SubjectTeacher.education_subject_id","matchTo": "SubjectTeacher.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${Principal.user.name}, ${Principal.user.preferred_name}, ${Principal.user.gender_id}</t>
+  </si>
+  <si>
+    <t>${InstitutionClasses.staff.name},${InstitutionClasses.staff.preferred_name},${InstitutionClasses.staff.gender_id}</t>
   </si>
 </sst>
 </file>
@@ -537,36 +542,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -631,7 +608,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,7 +764,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -814,7 +816,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1018,7 +1020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
@@ -1033,741 +1037,741 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" ht="12" customHeight="1">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="22" t="s">
+      <c r="E9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="12" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="27"/>
+      <c r="D10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="22" t="s">
+      <c r="E10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" ht="12" customHeight="1">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="E14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
+      <c r="A16" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
+      <c r="A17" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
+      <c r="A18" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
+      <c r="A19" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
+      <c r="A20" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
+      <c r="A22" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" ht="12" customHeight="1">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="D23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="E23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="F23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="G23" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" ht="12" customHeight="1">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="D24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="E24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="F24" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="G24" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
+      <c r="A26" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
+      <c r="A27" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
+      <c r="A28" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" ht="12" customHeight="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A32" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>73</v>
+      <c r="A32" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B35" s="30"/>
+      <c r="B35" s="20"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>78</v>
+      <c r="A36" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1"/>
@@ -2773,7 +2777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
@@ -2786,61 +2790,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="A1" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="A3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="12" customHeight="1"/>
     <row r="5" spans="1:13" ht="12" customHeight="1"/>
@@ -3856,7 +3860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
@@ -3870,66 +3874,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="A1" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="A3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1"/>
     <row r="5" spans="1:14" ht="12" customHeight="1"/>
@@ -4945,7 +4949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -4964,83 +4968,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="A1" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="31" t="s">
+      <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="G2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="H2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
+      <c r="G3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="H3" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1"/>
     <row r="5" spans="1:15" ht="12" customHeight="1"/>
@@ -6056,8 +6060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
@@ -6067,113 +6071,125 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="16" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="16" width="10.33203125" customWidth="1"/>
     <col min="17" max="27" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="A1" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="A2" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="E4" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="F4" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="G4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="H4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1"/>
     <row r="6" spans="1:17" ht="12" customHeight="1"/>
@@ -7177,7 +7193,7 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -7189,7 +7205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
@@ -7203,66 +7219,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="A1" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="A3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1"/>
     <row r="5" spans="1:14" ht="12" customHeight="1"/>
@@ -8278,7 +8294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
@@ -8293,75 +8309,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="A1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1"/>
     <row r="5" spans="1:15" ht="12" customHeight="1"/>

</xml_diff>

<commit_message>
POCOR-5054: code enahnce for showing modified user in report_card_template | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -415,13 +415,16 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "InstitutionStudentsReportCardsComments.security_user_name","rows": {"matchFrom": "AssessmentItems.education_subject_id","matchTo": "InstitutionStudentsReportCardsComments.education_subject_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "AssessmentItemResults.marks_formatted","type":"number","format":"2","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.education_subject_id","matchTo": "AssessmentItemResults.education_subject_id"},"columns": {"matchFrom": "AssessmentPeriods.id","matchTo": "AssessmentItemResults.assessment_period_id"}}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -469,6 +472,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -549,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -627,6 +636,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -646,8 +658,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1296,10 +1308,10 @@
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
@@ -1420,11 +1432,11 @@
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1441,10 +1453,10 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="30"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="16" t="s">
         <v>42</v>
       </c>
@@ -1464,10 +1476,10 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="30"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="16" t="s">
         <v>44</v>
       </c>
@@ -1487,10 +1499,10 @@
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="16" t="s">
         <v>46</v>
       </c>
@@ -1510,10 +1522,10 @@
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="16" t="s">
         <v>48</v>
       </c>
@@ -1552,15 +1564,15 @@
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1658,15 +1670,15 @@
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1679,17 +1691,17 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1702,17 +1714,17 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1745,11 +1757,11 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
@@ -2804,11 +2816,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -3888,12 +3900,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -4982,16 +4994,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -6075,7 +6087,7 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="G1:H1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -6091,14 +6103,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -6111,14 +6123,14 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -6177,16 +6189,18 @@
       <c r="C4" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="G4" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
         <v>125</v>
       </c>
@@ -7229,12 +7243,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -8319,14 +8333,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>

</xml_diff>

<commit_message>
POCOR-5054: Updated xls file upload | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -497,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -553,6 +553,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -569,7 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,12 +591,11 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -624,13 +632,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -642,7 +650,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -655,10 +663,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1063,7 +1074,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -1084,14 +1095,14 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A2" s="26"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="5"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1105,7 +1116,7 @@
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A3" s="26"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1146,17 +1157,16 @@
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="10"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1173,17 +1183,16 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="10"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1200,17 +1209,17 @@
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1227,17 +1236,17 @@
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1254,17 +1263,17 @@
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1281,17 +1290,17 @@
       <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="27"/>
+      <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1308,17 +1317,17 @@
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1335,17 +1344,17 @@
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1362,17 +1371,17 @@
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="27"/>
+      <c r="D13" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1389,17 +1398,17 @@
       <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="11" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="13"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1413,13 +1422,13 @@
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1432,15 +1441,15 @@
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1453,17 +1462,17 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="12" customHeight="1">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="16" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1476,17 +1485,17 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1499,17 +1508,17 @@
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" ht="12" customHeight="1">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1522,17 +1531,17 @@
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="12" customHeight="1">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -1545,13 +1554,13 @@
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" ht="16.5" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1564,15 +1573,15 @@
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="12" customHeight="1">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1585,25 +1594,25 @@
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" ht="12" customHeight="1">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="17" t="s">
         <v>56</v>
       </c>
       <c r="H23" s="4"/>
@@ -1618,25 +1627,25 @@
       <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" ht="12" customHeight="1">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="18" t="s">
         <v>63</v>
       </c>
       <c r="H24" s="4"/>
@@ -1651,13 +1660,13 @@
       <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1670,15 +1679,15 @@
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="12" customHeight="1">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1691,17 +1700,17 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="12" customHeight="1">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1714,17 +1723,17 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="12" customHeight="1">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="33" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1757,46 +1766,46 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B35" s="20"/>
+      <c r="B35" s="19"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="18" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2816,11 +2825,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -2833,13 +2842,13 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="12" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="4"/>
@@ -2854,11 +2863,11 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="22" t="s">
         <v>81</v>
       </c>
       <c r="D3" s="4"/>
@@ -3900,12 +3909,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -3918,16 +3927,16 @@
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="4"/>
@@ -3942,12 +3951,12 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="4"/>
@@ -4994,16 +5003,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -5013,28 +5022,28 @@
       <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>91</v>
       </c>
       <c r="I2" s="4"/>
@@ -5046,22 +5055,22 @@
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>96</v>
       </c>
       <c r="I3" s="4"/>
@@ -6087,7 +6096,7 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -6106,14 +6115,14 @@
       <c r="A1" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -6126,14 +6135,14 @@
       <c r="A2" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -6143,31 +6152,31 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>124</v>
       </c>
       <c r="J3" s="4"/>
@@ -6180,25 +6189,25 @@
       <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>108</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -7213,8 +7222,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7243,12 +7252,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -7261,16 +7270,16 @@
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="4"/>
@@ -7285,12 +7294,12 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
         <v>112</v>
       </c>
       <c r="E3" s="4"/>
@@ -8333,14 +8342,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -8352,22 +8361,22 @@
       <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>114</v>
       </c>
       <c r="G2" s="4"/>
@@ -8381,16 +8390,16 @@
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>117</v>
       </c>
       <c r="G3" s="4"/>

</xml_diff>

<commit_message>
POCOR-7424: Deleted empty three rows in excel, status:done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -646,7 +646,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -787,14 +787,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -902,11 +894,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.37"/>
@@ -1743,48 +1735,39 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="35"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="35"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="35"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="36"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="37"/>
+      <c r="A47" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="38"/>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>97</v>
-      </c>
-    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2731,9 +2714,9 @@
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="26">
@@ -2762,7 +2745,7 @@
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A44:B44"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2785,7 +2768,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.62"/>
@@ -2813,13 +2796,13 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="5"/>
@@ -2838,7 +2821,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="27"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="38" t="s">
         <v>102</v>
       </c>
       <c r="D3" s="5"/>
@@ -3874,7 +3857,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
@@ -3904,16 +3887,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="5"/>
@@ -4969,7 +4952,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
@@ -5003,28 +4986,28 @@
       <c r="O1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="35" t="s">
         <v>112</v>
       </c>
       <c r="I2" s="5"/>
@@ -6084,7 +6067,7 @@
       <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11"/>
@@ -6117,17 +6100,17 @@
       <c r="P1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -6137,10 +6120,10 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -6183,7 +6166,7 @@
       <c r="C4" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="41" t="s">
         <v>132</v>
       </c>
       <c r="E4" s="27" t="s">
@@ -7231,7 +7214,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
@@ -7261,16 +7244,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="5"/>
@@ -8326,7 +8309,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
@@ -8358,22 +8341,22 @@
       <c r="O1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="35" t="s">
         <v>143</v>
       </c>
       <c r="G2" s="5"/>

</xml_diff>

<commit_message>
report card xlsx update||new placeholder
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/report_card_template.xlsx
+++ b/webroot/export/customexcel/default_templates/report_card_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="149">
   <si>
     <t xml:space="preserve">${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t xml:space="preserve">${InstitutionStudentsReportCards.student.body_mass_index}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${InstitutionStudentsReportCards.gpa}</t>
   </si>
   <si>
     <t xml:space="preserve">Gender:</t>
@@ -894,11 +900,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.37"/>
@@ -1259,14 +1265,18 @@
       <c r="Q14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="C15" s="10"/>
       <c r="D15" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="19"/>
@@ -1302,7 +1312,7 @@
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
@@ -1323,11 +1333,11 @@
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18" s="22"/>
       <c r="C18" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -1346,11 +1356,11 @@
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B19" s="22"/>
       <c r="C19" s="23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -1369,11 +1379,11 @@
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -1392,11 +1402,11 @@
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -1434,7 +1444,7 @@
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -1455,25 +1465,25 @@
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1488,25 +1498,25 @@
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1540,7 +1550,7 @@
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
@@ -1561,11 +1571,11 @@
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="29" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
@@ -1584,11 +1594,11 @@
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
@@ -1627,31 +1637,31 @@
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1663,17 +1673,17 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="31"/>
@@ -1684,48 +1694,48 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G41" s="26" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D42" s="33" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G42" s="33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -1736,33 +1746,33 @@
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="35" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B44" s="35"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C46" s="36"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="27" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2749,7 +2759,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -2768,19 +2778,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="7" style="0" width="10.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -2797,13 +2807,13 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2818,11 +2828,11 @@
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3838,7 +3848,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -3857,20 +3867,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="0" width="10.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -3888,16 +3898,16 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -3912,12 +3922,12 @@
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -4933,7 +4943,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -4952,11 +4962,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.11"/>
@@ -4968,7 +4978,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -4987,28 +4997,28 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -5020,22 +5030,22 @@
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -6048,7 +6058,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -6067,21 +6077,21 @@
       <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="8" style="0" width="10.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="17" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -6101,7 +6111,7 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -6121,31 +6131,31 @@
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -6158,31 +6168,31 @@
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -7195,7 +7205,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -7214,20 +7224,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="0" width="10.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -7245,16 +7255,16 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -7269,12 +7279,12 @@
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -8290,7 +8300,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -8309,11 +8319,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.61"/>
@@ -8323,7 +8333,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -8342,22 +8352,22 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -8371,16 +8381,16 @@
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -9395,7 +9405,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>